<commit_message>
commit before reset on laptop, copied the figures and evaluation.tex
</commit_message>
<xml_diff>
--- a/dataset/experiments-cases-design-weight.xlsx
+++ b/dataset/experiments-cases-design-weight.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="generate-weights_test" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t xml:space="preserve">WeightName</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Case ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weightKeep2</t>
   </si>
 </sst>
 </file>
@@ -136,13 +139,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -164,8 +171,8 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2581,10 +2588,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2602,7 +2609,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2616,7 +2626,10 @@
       <c r="C2" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
+        <v>0.0975373359203966</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -2630,7 +2643,10 @@
       <c r="C3" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
+        <v>0.426216532321556</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -2644,7 +2660,10 @@
       <c r="C4" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
+        <v>0.636270697849109</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -2655,7 +2674,10 @@
       <c r="C5" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
+        <v>0.818623193631408</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2666,37 +2688,40 @@
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
+        <v>0.839010519465712</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="n">
+      <c r="E11" s="0" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
after report to Bas need to code one plugin
</commit_message>
<xml_diff>
--- a/dataset/experiments-cases-design-weight.xlsx
+++ b/dataset/experiments-cases-design-weight.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="generate-weights_test" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="datanoise-rate" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="weigths-sample" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="generate-weights" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="generate-weights-more-distance" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="generate-weights_test" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="datanoise-rate" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="weigths-sample" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="generate-weights" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
   <si>
     <t xml:space="preserve">WeightName</t>
   </si>
   <si>
     <t xml:space="preserve">caseID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weightKeep</t>
   </si>
   <si>
     <t xml:space="preserve">weightVar</t>
@@ -44,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">Neg-weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weightKeep</t>
   </si>
   <si>
     <t xml:space="preserve">testID</t>
@@ -169,6 +170,150 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -188,15 +333,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -210,7 +355,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -224,7 +369,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -238,7 +383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -268,13 +413,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,7 +1169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1045,13 +1190,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,15 +2728,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2607,18 +2752,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2635,7 +2780,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -2652,7 +2797,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
change the demo data
</commit_message>
<xml_diff>
--- a/dataset/experiments-cases-design-weight.xlsx
+++ b/dataset/experiments-cases-design-weight.xlsx
@@ -9,10 +9,11 @@
   </bookViews>
   <sheets>
     <sheet name="generate-weights-more-distance" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="generate-weights-reallife" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="datanoise-rate" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="weigths-sample" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="generate-weights" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="generate-weights-reallife_2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="generate-weights-reallife" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="datanoise-rate" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="weigths-sample" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="generate-weights" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="14">
   <si>
     <t xml:space="preserve">WeightName</t>
   </si>
@@ -314,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,10 +362,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,10 +376,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,10 +387,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,20 +398,9 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -426,6 +416,122 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1211,7 +1317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2770,7 +2876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>